<commit_message>
Update Business intelligence systems - System Development - BI Project - Finance Systems - AFS Data Specification V4.55.xlsx
WIP for AFS
</commit_message>
<xml_diff>
--- a/specifications/afs/Business intelligence systems - System Development - BI Project - Finance Systems - AFS Data Specification V4.55.xlsx
+++ b/specifications/afs/Business intelligence systems - System Development - BI Project - Finance Systems - AFS Data Specification V4.55.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\afs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3701D989-D70F-4463-A4A9-97800EB42E1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DAB082-BB43-4055-AE99-DAECB958F433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4243" uniqueCount="2307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4245" uniqueCount="2309">
   <si>
     <t>Revision History</t>
   </si>
@@ -7216,6 +7216,12 @@
   <si>
     <t>numeric(9,0,negative)</t>
   </si>
+  <si>
+    <t>Total key management personnel emoluments is not greater than Chief Executive emoluments.  Please provide a comment.</t>
+  </si>
+  <si>
+    <t>Deferred income is not split between amounts due within 1 year and amounts due outwith 1 year. Please enter a comment at Total deferred income: amounts falling due after more than one year.</t>
+  </si>
 </sst>
 </file>
 
@@ -7226,7 +7232,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0;\(#,##0.0\)"/>
     <numFmt numFmtId="166" formatCode="#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="56" x14ac:knownFonts="1">
+  <fonts count="57" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7579,6 +7585,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -7989,7 +8001,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="295">
+  <cellXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8788,6 +8800,7 @@
     <xf numFmtId="0" fontId="18" fillId="18" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11103,7 +11116,9 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:XFB23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11466,7 +11481,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -14094,12 +14109,12 @@
   </sheetPr>
   <dimension ref="A1:AH640"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B520" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="I162" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="B6" sqref="B6"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A523" sqref="A523"/>
+      <selection pane="bottomRight" activeCell="O168" sqref="O168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -22332,8 +22347,13 @@
         <v>841</v>
       </c>
       <c r="M167" s="47"/>
-      <c r="N167" s="39"/>
-      <c r="O167" s="47"/>
+      <c r="N167" s="295" t="b">
+        <f>OR((I135 + I144=0),AND(I135&lt;0,I144&lt;=0),(H167&lt;&gt;""))</f>
+        <v>1</v>
+      </c>
+      <c r="O167" s="47" t="s">
+        <v>2308</v>
+      </c>
       <c r="P167" s="36"/>
       <c r="Q167" s="152"/>
       <c r="R167" s="36"/>
@@ -37833,9 +37853,13 @@
         <v>841</v>
       </c>
       <c r="M481" s="47"/>
-      <c r="N481" s="39"/>
-      <c r="O481" s="47"/>
-      <c r="P481" s="36"/>
+      <c r="N481" s="47" t="b">
+        <f>OR(H459&lt;H460,H481&lt;&gt;"")</f>
+        <v>1</v>
+      </c>
+      <c r="O481" s="36" t="s">
+        <v>2307</v>
+      </c>
       <c r="Q481" s="152"/>
       <c r="R481" s="36"/>
       <c r="S481" s="152"/>

</xml_diff>